<commit_message>
Ga: add new feature
</commit_message>
<xml_diff>
--- a/cqc-support/src/main/webapp/resources/template/型式试验结果.xlsx
+++ b/cqc-support/src/main/webapp/resources/template/型式试验结果.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B545591-41C0-4E6E-9309-AAC5428522EE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>试验项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,6 +43,10 @@
   </si>
   <si>
     <t>类型(零部件/原材料)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -385,19 +390,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="6" width="15.58203125" customWidth="1"/>
+    <col min="7" max="7" width="30.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -415,10 +421,18 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{FFFCB290-3F97-4086-AF79-57A97917A7E6}">
+      <formula1>"零部件,原材料"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>